<commit_message>
comprension de la matrice merice
</commit_message>
<xml_diff>
--- a/FOAD/Merise/Cours_exemples/fiche_intervention.xlsx
+++ b/FOAD/Merise/Cours_exemples/fiche_intervention.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jonat\Documents\GitHub\CRM\CDA_2005\FOAD\Merise\Cours_exemples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBCDDE0-291E-4D4B-8724-843EB33C64F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dictionnaire" sheetId="1" r:id="rId1"/>
+    <sheet name="Matrice" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +25,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>intervention</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>adresse</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>depart</t>
+  </si>
+  <si>
+    <t>arrivee</t>
+  </si>
+  <si>
+    <t>intervenant</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>observation</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +74,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +102,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +414,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8023AF6F-6221-4808-A9B3-416DC164A565}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="5" width="11.5546875" style="4"/>
+    <col min="6" max="13" width="11.5546875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="F1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>